<commit_message>
Adding changes for stored sheets
</commit_message>
<xml_diff>
--- a/app/uploads/ucsd13.xlsx
+++ b/app/uploads/ucsd13.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFF0A56E-D4D0-41B2-9DB9-1739D1EE0475}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swapnilpatil/Files/College/Spring Quarter 20/Neatlabs/OneDrive_1_5-26-2020/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E08FDA-4956-1842-8B88-9D0A4F266544}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="weekly_summary" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -166,7 +171,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,9 +570,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +634,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -694,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -747,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -800,7 +805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -865,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -930,7 +935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -995,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1060,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1125,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1178,7 +1183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1243,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1308,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1373,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1438,7 +1443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1503,7 +1508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1568,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1633,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1698,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1763,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1828,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -1893,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1958,7 +1963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -2023,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -2088,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -2153,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Adding excel files and compatibility
</commit_message>
<xml_diff>
--- a/app/uploads/ucsd13.xlsx
+++ b/app/uploads/ucsd13.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22920"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swapnilpatil/Files/College/Spring Quarter 20/Neatlabs/OneDrive_1_5-26-2020/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E08FDA-4956-1842-8B88-9D0A4F266544}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_FFC65FC028A1A9FC3E170BB7E349BAE74C82CC45" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="weekly_summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -171,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,9 +565,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -699,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -752,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -805,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -870,7 +865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -935,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1000,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1065,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1130,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1183,7 +1178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1248,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1313,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1378,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1443,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1508,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1573,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1638,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1703,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1768,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1833,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -1898,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1963,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -2028,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -2093,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -2158,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>

</xml_diff>